<commit_message>
prepearing data for whole catchment
</commit_message>
<xml_diff>
--- a/South_Valley/data/south_valley_morphology_data.xlsx
+++ b/South_Valley/data/south_valley_morphology_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
   <si>
     <t>1</t>
   </si>
@@ -208,6 +208,21 @@
   </si>
   <si>
     <t>0.22</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>mor</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>mix</t>
   </si>
 </sst>
 </file>
@@ -555,16 +570,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR33"/>
+  <dimension ref="A1:AS34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG3" sqref="AG3:AG33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -574,147 +589,147 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="E2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>47</v>
@@ -735,10 +750,10 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>47</v>
@@ -753,10 +768,10 @@
         <v>47</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>47</v>
@@ -765,7 +780,7 @@
         <v>47</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>49</v>
@@ -794,8 +809,8 @@
       <c r="AG2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>50</v>
+      <c r="AH2" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>50</v>
@@ -827,8 +842,11 @@
       <c r="AR2" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AS2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -838,56 +856,59 @@
       <c r="C3">
         <v>43.220208</v>
       </c>
-      <c r="E3">
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3">
         <v>6.73</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>228.2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.63</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.3</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>2.5099999999999998</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.1</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>0.2</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>0.5</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>1.8</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>4</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>0</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>1</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>53</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>11</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -897,56 +918,59 @@
       <c r="C4">
         <v>43.220910000000003</v>
       </c>
-      <c r="E4">
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4">
         <v>5.14</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>154.6</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3.25</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.2</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.3</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>10.11</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0.3</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0.2</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>0.8</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>6</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>51</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>0</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>57</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>12</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -956,65 +980,68 @@
       <c r="C5">
         <v>43.220357999999898</v>
       </c>
-      <c r="E5">
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5">
         <v>6.66</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>291.60000000000002</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5.48</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.23</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.2</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.2</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.53</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.1</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>0.17</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>0.3</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>0.6</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>0.11</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>0.3</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>5</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>0</v>
       </c>
       <c r="AJ5" t="s">
         <v>0</v>
       </c>
-      <c r="AL5">
+      <c r="AK5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM5">
         <v>55</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>10</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1024,62 +1051,65 @@
       <c r="C6">
         <v>43.220919000000002</v>
       </c>
-      <c r="E6">
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6">
         <v>1.36</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>419.2</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.52</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.13</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.21</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.1</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.39</v>
-      </c>
-      <c r="Q6">
-        <v>0.1</v>
       </c>
       <c r="R6">
         <v>0.1</v>
       </c>
       <c r="S6">
+        <v>0.1</v>
+      </c>
+      <c r="T6">
         <v>0.26</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>0.2</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>0.3</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>11</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>0</v>
       </c>
       <c r="AJ6" t="s">
         <v>0</v>
       </c>
-      <c r="AL6">
+      <c r="AK6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM6">
         <v>61</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>5</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1089,62 +1119,65 @@
       <c r="C7">
         <v>43.220782</v>
       </c>
-      <c r="E7">
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7">
         <v>11.8</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>240.5</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.5</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>9.84</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.22</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1.1399999999999999</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>1.02</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>6.84</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>0.5</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>0.4</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>1.7</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>0.5</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <v>12</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>1</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>52</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>43</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>18</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1154,1714 +1187,1764 @@
       <c r="C8">
         <v>43.220412000000003</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8">
         <v>0.51</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>8.1199999999999992</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>300.39999999999998</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1.5</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>8.8000000000000007</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1.31</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0.67</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0.3</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0.9</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>2.65</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.2</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.1</v>
-      </c>
-      <c r="R8">
-        <v>0.2</v>
       </c>
       <c r="S8">
         <v>0.2</v>
       </c>
       <c r="T8">
+        <v>0.2</v>
+      </c>
+      <c r="U8">
         <v>0.1</v>
-      </c>
-      <c r="U8">
-        <v>0.5</v>
       </c>
       <c r="V8">
         <v>0.5</v>
       </c>
       <c r="W8">
+        <v>0.5</v>
+      </c>
+      <c r="X8">
         <v>1.8</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>0.4</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>9</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>52</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AK8" t="s">
         <v>0</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>45</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>16</v>
       </c>
-      <c r="AN8">
+      <c r="AO8">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>42.467429000000003</v>
+      </c>
+      <c r="C9">
+        <v>43.220792000000003</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>5.57</v>
+      </c>
+      <c r="G9">
+        <v>185.3</v>
+      </c>
+      <c r="H9">
+        <v>1.9</v>
+      </c>
+      <c r="I9">
+        <v>3.1</v>
+      </c>
+      <c r="J9">
+        <v>2.1</v>
+      </c>
+      <c r="K9">
+        <v>3.87</v>
+      </c>
+      <c r="L9">
+        <v>2.11</v>
+      </c>
+      <c r="M9">
+        <v>6.17</v>
+      </c>
+      <c r="O9">
+        <v>1.4</v>
+      </c>
+      <c r="P9">
+        <v>7.66</v>
+      </c>
+      <c r="T9">
+        <v>0.6</v>
+      </c>
+      <c r="W9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X9">
+        <v>1.6</v>
+      </c>
+      <c r="AH9">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AI9">
+        <v>11</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>40</v>
+      </c>
+      <c r="AN9">
+        <v>23</v>
+      </c>
+      <c r="AO9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>42.467657000000003</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>43.220773999999899</v>
       </c>
-      <c r="D9">
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10">
         <v>0.59</v>
       </c>
-      <c r="E9">
+      <c r="F10">
         <v>8.0299999999999994</v>
       </c>
-      <c r="F9">
+      <c r="G10">
         <v>256.60000000000002</v>
       </c>
-      <c r="H9">
+      <c r="I10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J9">
+      <c r="K10">
         <v>7.66</v>
       </c>
-      <c r="K9">
+      <c r="L10">
         <v>1.05</v>
       </c>
-      <c r="L9">
+      <c r="M10">
         <v>0.42</v>
       </c>
-      <c r="M9">
+      <c r="N10">
         <v>0.1</v>
       </c>
-      <c r="N9">
+      <c r="O10">
         <v>0.7</v>
       </c>
-      <c r="O9">
+      <c r="P10">
         <v>3.48</v>
       </c>
-      <c r="S9">
+      <c r="T10">
         <v>0.3</v>
       </c>
-      <c r="V9">
+      <c r="W10">
         <v>0.4</v>
       </c>
-      <c r="W9">
+      <c r="X10">
         <v>1.5</v>
       </c>
-      <c r="Z9">
+      <c r="AA10">
         <v>0.11</v>
       </c>
-      <c r="AB9">
+      <c r="AC10">
         <v>0.8</v>
       </c>
-      <c r="AH9">
+      <c r="AI10">
         <v>11</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AJ10" t="s">
         <v>0</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK10" t="s">
         <v>51</v>
       </c>
-      <c r="AL9">
+      <c r="AM10">
         <v>46</v>
       </c>
-      <c r="AM9">
+      <c r="AN10">
         <v>18</v>
       </c>
-      <c r="AN9">
+      <c r="AO10">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>42.467986000000003</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>43.220382999999899</v>
       </c>
-      <c r="D10">
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11">
         <v>0.21</v>
       </c>
-      <c r="E10">
+      <c r="F11">
         <v>4.0599999999999996</v>
       </c>
-      <c r="F10">
+      <c r="G11">
         <v>201.65</v>
       </c>
-      <c r="H10">
+      <c r="I11">
         <v>1.2</v>
       </c>
-      <c r="J10">
+      <c r="K11">
         <v>8.4600000000000009</v>
       </c>
-      <c r="K10">
+      <c r="L11">
         <v>0.6</v>
       </c>
-      <c r="L10">
+      <c r="M11">
         <v>0.25</v>
       </c>
-      <c r="M10">
+      <c r="N11">
         <v>0.1</v>
       </c>
-      <c r="N10">
+      <c r="O11">
         <v>0.3</v>
       </c>
-      <c r="O10">
+      <c r="P11">
         <v>3.23</v>
       </c>
-      <c r="P10">
+      <c r="Q11">
         <v>0.3</v>
       </c>
-      <c r="Q10">
+      <c r="R11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="R10">
+      <c r="S11">
         <v>0.4</v>
       </c>
-      <c r="S10">
+      <c r="T11">
         <v>0.3</v>
-      </c>
-      <c r="V10">
-        <v>0.7</v>
-      </c>
-      <c r="W10">
-        <v>2.1</v>
-      </c>
-      <c r="AH10">
-        <v>8</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL10">
-        <v>65</v>
-      </c>
-      <c r="AM10">
-        <v>5</v>
-      </c>
-      <c r="AN10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>42.468632999999897</v>
-      </c>
-      <c r="C11">
-        <v>43.220460000000003</v>
-      </c>
-      <c r="E11">
-        <v>6.49</v>
-      </c>
-      <c r="F11">
-        <v>170.6</v>
-      </c>
-      <c r="H11">
-        <v>1.5</v>
-      </c>
-      <c r="J11">
-        <v>2.54</v>
-      </c>
-      <c r="K11">
-        <v>0.96</v>
-      </c>
-      <c r="L11">
-        <v>1.58</v>
-      </c>
-      <c r="M11">
-        <v>0.2</v>
-      </c>
-      <c r="N11">
-        <v>1.3</v>
-      </c>
-      <c r="O11">
-        <v>10.77</v>
-      </c>
-      <c r="S11">
-        <v>0.2</v>
-      </c>
-      <c r="V11">
-        <v>1.1000000000000001</v>
       </c>
       <c r="W11">
         <v>0.7</v>
       </c>
-      <c r="Y11">
-        <v>0.5</v>
-      </c>
-      <c r="AH11">
-        <v>7</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL11">
-        <v>50</v>
+      <c r="X11">
+        <v>2.1</v>
+      </c>
+      <c r="AI11">
+        <v>8</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>52</v>
       </c>
       <c r="AM11">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="AN11">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="AO11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>42.469019000000003</v>
+        <v>42.468632999999897</v>
       </c>
       <c r="C12">
-        <v>43.221048000000003</v>
-      </c>
-      <c r="E12">
-        <v>2.23</v>
+        <v>43.220460000000003</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
       </c>
       <c r="F12">
-        <v>270</v>
-      </c>
-      <c r="J12">
-        <v>2.21</v>
+        <v>6.49</v>
+      </c>
+      <c r="G12">
+        <v>170.6</v>
+      </c>
+      <c r="I12">
+        <v>1.5</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>2.54</v>
       </c>
       <c r="L12">
-        <v>0.86</v>
+        <v>0.96</v>
       </c>
       <c r="M12">
+        <v>1.58</v>
+      </c>
+      <c r="N12">
         <v>0.2</v>
       </c>
-      <c r="N12">
-        <v>0.4</v>
-      </c>
       <c r="O12">
-        <v>1.46</v>
-      </c>
-      <c r="S12">
-        <v>0.3</v>
-      </c>
-      <c r="V12">
-        <v>0.5</v>
+        <v>1.3</v>
+      </c>
+      <c r="P12">
+        <v>10.77</v>
+      </c>
+      <c r="T12">
+        <v>0.2</v>
       </c>
       <c r="W12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Y12">
+      <c r="X12">
+        <v>0.7</v>
+      </c>
+      <c r="Z12">
+        <v>0.5</v>
+      </c>
+      <c r="AI12">
+        <v>7</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM12">
+        <v>50</v>
+      </c>
+      <c r="AN12">
+        <v>8</v>
+      </c>
+      <c r="AO12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>42.469019000000003</v>
+      </c>
+      <c r="C13">
+        <v>43.221048000000003</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>2.23</v>
+      </c>
+      <c r="G13">
+        <v>270</v>
+      </c>
+      <c r="K13">
+        <v>2.21</v>
+      </c>
+      <c r="L13">
+        <v>0.5</v>
+      </c>
+      <c r="M13">
+        <v>0.86</v>
+      </c>
+      <c r="N13">
+        <v>0.2</v>
+      </c>
+      <c r="O13">
+        <v>0.4</v>
+      </c>
+      <c r="P13">
+        <v>1.46</v>
+      </c>
+      <c r="T13">
+        <v>0.3</v>
+      </c>
+      <c r="W13">
+        <v>0.5</v>
+      </c>
+      <c r="X13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z13">
         <v>0.15</v>
       </c>
-      <c r="AB12">
+      <c r="AC13">
         <v>0.5</v>
       </c>
-      <c r="AH12">
+      <c r="AI13">
         <v>11</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AJ13" t="s">
         <v>0</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AK13" t="s">
         <v>51</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL13" t="s">
         <v>1</v>
       </c>
-      <c r="AL12">
+      <c r="AM13">
         <v>55</v>
       </c>
-      <c r="AM12">
+      <c r="AN13">
         <v>14</v>
       </c>
-      <c r="AN12">
+      <c r="AO13">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>42.4700279999999</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>43.220308000000003</v>
       </c>
-      <c r="E13">
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14">
         <v>7.18</v>
       </c>
-      <c r="F13">
+      <c r="G14">
         <v>207.3</v>
       </c>
-      <c r="G13">
+      <c r="H14">
         <v>0.3</v>
       </c>
-      <c r="H13">
+      <c r="I14">
         <v>0.21</v>
       </c>
-      <c r="J13">
+      <c r="K14">
         <v>3.99</v>
       </c>
-      <c r="K13">
+      <c r="L14">
         <v>0.9</v>
       </c>
-      <c r="L13">
+      <c r="M14">
         <v>0.71</v>
       </c>
-      <c r="N13">
+      <c r="O14">
         <v>1.2</v>
       </c>
-      <c r="O13">
+      <c r="P14">
         <v>8.61</v>
       </c>
-      <c r="S13">
+      <c r="T14">
         <v>0.5</v>
       </c>
-      <c r="V13">
+      <c r="W14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W13">
+      <c r="X14">
         <v>1.3</v>
       </c>
-      <c r="AH13">
+      <c r="AI14">
         <v>9</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AJ14" t="s">
         <v>1</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AK14" t="s">
         <v>54</v>
       </c>
-      <c r="AK13" t="s">
+      <c r="AL14" t="s">
         <v>0</v>
       </c>
-      <c r="AL13">
+      <c r="AM14">
         <v>41</v>
       </c>
-      <c r="AM13">
+      <c r="AN14">
         <v>10</v>
       </c>
-      <c r="AN13">
+      <c r="AO14">
         <v>34</v>
       </c>
-      <c r="AO13" t="s">
+      <c r="AP14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>42.470640000000003</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>43.219876999999897</v>
       </c>
-      <c r="D14">
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15">
         <v>1.31</v>
       </c>
-      <c r="E14">
+      <c r="F15">
         <v>8.9700000000000006</v>
       </c>
-      <c r="F14">
+      <c r="G15">
         <v>277.5</v>
       </c>
-      <c r="G14">
+      <c r="H15">
         <v>0.46</v>
       </c>
-      <c r="H14">
+      <c r="I15">
         <v>0.18</v>
       </c>
-      <c r="I14">
+      <c r="J15">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J14">
+      <c r="K15">
         <v>6.56</v>
       </c>
-      <c r="K14">
+      <c r="L15">
         <v>1.3</v>
       </c>
-      <c r="L14">
+      <c r="M15">
         <v>0.79</v>
       </c>
-      <c r="M14">
+      <c r="N15">
         <v>0.2</v>
       </c>
-      <c r="N14">
+      <c r="O15">
         <v>0.7</v>
       </c>
-      <c r="O14">
+      <c r="P15">
         <v>5.17</v>
       </c>
-      <c r="S14">
+      <c r="T15">
         <v>0.16</v>
       </c>
-      <c r="V14">
+      <c r="W15">
         <v>0.6</v>
       </c>
-      <c r="W14">
+      <c r="X15">
         <v>1.6</v>
       </c>
-      <c r="AE14">
+      <c r="AF15">
         <v>1.4</v>
       </c>
-      <c r="AF14">
+      <c r="AG15">
         <v>0.1</v>
       </c>
-      <c r="AH14">
+      <c r="AI15">
         <v>7</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AK15" t="s">
         <v>55</v>
       </c>
-      <c r="AL14">
+      <c r="AM15">
         <v>42</v>
       </c>
-      <c r="AM14">
+      <c r="AN15">
         <v>7</v>
       </c>
-      <c r="AN14">
+      <c r="AO15">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>42.472442000000001</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>43.2212719999999</v>
       </c>
-      <c r="E15">
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16">
         <v>5.87</v>
       </c>
-      <c r="F15">
+      <c r="G16">
         <v>167.4</v>
       </c>
-      <c r="G15">
+      <c r="H16">
         <v>0.21</v>
       </c>
-      <c r="H15">
+      <c r="I16">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I15">
+      <c r="J16">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J15">
+      <c r="K16">
         <v>2.41</v>
       </c>
-      <c r="K15">
+      <c r="L16">
         <v>0.98</v>
       </c>
-      <c r="L15">
+      <c r="M16">
         <v>0.65</v>
       </c>
-      <c r="N15">
+      <c r="O16">
         <v>1.4</v>
       </c>
-      <c r="O15">
+      <c r="P16">
         <v>9.3699999999999992</v>
       </c>
-      <c r="S15">
+      <c r="T16">
         <v>1.4</v>
       </c>
-      <c r="V15">
+      <c r="W16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W15">
+      <c r="X16">
         <v>1.6</v>
       </c>
-      <c r="Z15">
+      <c r="AA16">
         <v>0.48</v>
       </c>
-      <c r="AH15">
+      <c r="AI16">
         <v>14</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AK16" t="s">
         <v>56</v>
       </c>
-      <c r="AL15">
+      <c r="AM16">
         <v>31</v>
       </c>
-      <c r="AM15">
+      <c r="AN16">
         <v>8</v>
       </c>
-      <c r="AN15">
+      <c r="AO16">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>42.472571000000002</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>43.220233999999898</v>
       </c>
-      <c r="E16">
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17">
         <v>10.210000000000001</v>
       </c>
-      <c r="F16">
+      <c r="G17">
         <v>304.7</v>
       </c>
-      <c r="G16">
+      <c r="H17">
         <v>0.18</v>
       </c>
-      <c r="H16">
+      <c r="I17">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J16">
+      <c r="K17">
         <v>6.31</v>
       </c>
-      <c r="K16">
+      <c r="L17">
         <v>3.32</v>
       </c>
-      <c r="L16">
+      <c r="M17">
         <v>1.17</v>
       </c>
-      <c r="N16">
+      <c r="O17">
         <v>1.3</v>
       </c>
-      <c r="O16">
+      <c r="P17">
         <v>7.14</v>
       </c>
-      <c r="P16">
+      <c r="Q17">
         <v>0.7</v>
       </c>
-      <c r="S16">
+      <c r="T17">
         <v>0.3</v>
       </c>
-      <c r="V16">
+      <c r="W17">
         <v>0.7</v>
       </c>
-      <c r="W16">
+      <c r="X17">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AH16">
+      <c r="AI17">
         <v>3</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AK17" t="s">
         <v>53</v>
       </c>
-      <c r="AK16" t="s">
+      <c r="AL17" t="s">
         <v>0</v>
       </c>
-      <c r="AL16">
+      <c r="AM17">
         <v>45</v>
       </c>
-      <c r="AM16">
+      <c r="AN17">
         <v>3</v>
       </c>
-      <c r="AN16">
+      <c r="AO17">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>42.472641000000003</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>43.220311000000002</v>
       </c>
-      <c r="E17">
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
         <v>6.32</v>
       </c>
-      <c r="F17">
+      <c r="G18">
         <v>159.9</v>
       </c>
-      <c r="H17">
+      <c r="I18">
         <v>3</v>
       </c>
-      <c r="J17">
+      <c r="K18">
         <v>5.59</v>
       </c>
-      <c r="K17">
+      <c r="L18">
         <v>1.23</v>
       </c>
-      <c r="L17">
+      <c r="M18">
         <v>0.71</v>
       </c>
-      <c r="N17">
+      <c r="O18">
         <v>1</v>
       </c>
-      <c r="O17">
+      <c r="P18">
         <v>5.03</v>
       </c>
-      <c r="P17">
+      <c r="Q18">
         <v>0.3</v>
       </c>
-      <c r="S17">
+      <c r="T18">
         <v>0.5</v>
       </c>
-      <c r="V17">
+      <c r="W18">
         <v>0.7</v>
       </c>
-      <c r="W17">
+      <c r="X18">
         <v>1.9</v>
       </c>
-      <c r="AH17">
+      <c r="AI18">
         <v>6</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AK18" t="s">
         <v>51</v>
       </c>
-      <c r="AL17">
+      <c r="AM18">
         <v>57</v>
       </c>
-      <c r="AM17">
+      <c r="AN18">
         <v>14</v>
       </c>
-      <c r="AN17">
+      <c r="AO18">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>42.47448</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>43.219354000000003</v>
       </c>
-      <c r="E18">
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19">
         <v>8.3800000000000008</v>
       </c>
-      <c r="F18">
+      <c r="G19">
         <v>361.3</v>
       </c>
-      <c r="J18">
+      <c r="K19">
         <v>8.66</v>
       </c>
-      <c r="K18">
+      <c r="L19">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L18">
+      <c r="M19">
         <v>0.15</v>
       </c>
-      <c r="N18">
+      <c r="O19">
         <v>2</v>
       </c>
-      <c r="O18">
+      <c r="P19">
         <v>13.45</v>
       </c>
-      <c r="S18">
+      <c r="T19">
         <v>1</v>
       </c>
-      <c r="V18">
+      <c r="W19">
         <v>0.7</v>
       </c>
-      <c r="W18">
+      <c r="X19">
         <v>2.4</v>
       </c>
-      <c r="AH18">
+      <c r="AI19">
         <v>11</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AK19" t="s">
         <v>51</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AL19" t="s">
         <v>1</v>
       </c>
-      <c r="AL18">
+      <c r="AM19">
         <v>32</v>
       </c>
-      <c r="AM18">
+      <c r="AN19">
         <v>31</v>
       </c>
-      <c r="AN18">
+      <c r="AO19">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A19">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>42.474397000000003</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>43.218505</v>
       </c>
-      <c r="D19">
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E19">
+      <c r="F20">
         <v>5.4</v>
       </c>
-      <c r="F19">
+      <c r="G20">
         <v>138.4</v>
       </c>
-      <c r="J19">
+      <c r="K20">
         <v>5.66</v>
       </c>
-      <c r="K19">
+      <c r="L20">
         <v>0.16</v>
       </c>
-      <c r="L19">
+      <c r="M20">
         <v>0.49</v>
-      </c>
-      <c r="M19">
-        <v>0.3</v>
-      </c>
-      <c r="N19">
-        <v>0.6</v>
-      </c>
-      <c r="O19">
-        <v>3.35</v>
-      </c>
-      <c r="P19">
-        <v>0.4</v>
-      </c>
-      <c r="S19">
-        <v>0.3</v>
-      </c>
-      <c r="U19">
-        <v>1.02</v>
-      </c>
-      <c r="V19">
-        <v>0.7</v>
-      </c>
-      <c r="W19">
-        <v>1.5</v>
-      </c>
-      <c r="Y19">
-        <v>0.3</v>
-      </c>
-      <c r="AH19">
-        <v>9</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL19">
-        <v>50</v>
-      </c>
-      <c r="AM19">
-        <v>13</v>
-      </c>
-      <c r="AN19">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>42.474685999999899</v>
-      </c>
-      <c r="C20">
-        <v>43.2175879999999</v>
-      </c>
-      <c r="D20">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <v>234.5</v>
-      </c>
-      <c r="G20">
-        <v>0.9</v>
-      </c>
-      <c r="H20">
-        <v>0.7</v>
-      </c>
-      <c r="J20">
-        <v>4.83</v>
-      </c>
-      <c r="K20">
-        <v>0.71</v>
-      </c>
-      <c r="L20">
-        <v>0.35</v>
-      </c>
-      <c r="M20">
-        <v>0.1</v>
       </c>
       <c r="N20">
         <v>0.3</v>
       </c>
       <c r="O20">
-        <v>1.92</v>
-      </c>
-      <c r="R20">
-        <v>0.1</v>
-      </c>
-      <c r="S20">
-        <v>0.2</v>
-      </c>
-      <c r="U20">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
+      </c>
+      <c r="P20">
+        <v>3.35</v>
+      </c>
+      <c r="Q20">
+        <v>0.4</v>
+      </c>
+      <c r="T20">
+        <v>0.3</v>
       </c>
       <c r="V20">
-        <v>0.3</v>
+        <v>1.02</v>
       </c>
       <c r="W20">
         <v>0.7</v>
       </c>
-      <c r="AH20">
+      <c r="X20">
+        <v>1.5</v>
+      </c>
+      <c r="Z20">
+        <v>0.3</v>
+      </c>
+      <c r="AI20">
+        <v>9</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>50</v>
+      </c>
+      <c r="AN20">
+        <v>13</v>
+      </c>
+      <c r="AO20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>42.474685999999899</v>
+      </c>
+      <c r="C21">
+        <v>43.2175879999999</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>234.5</v>
+      </c>
+      <c r="H21">
+        <v>0.9</v>
+      </c>
+      <c r="I21">
+        <v>0.7</v>
+      </c>
+      <c r="K21">
+        <v>4.83</v>
+      </c>
+      <c r="L21">
+        <v>0.71</v>
+      </c>
+      <c r="M21">
+        <v>0.35</v>
+      </c>
+      <c r="N21">
+        <v>0.1</v>
+      </c>
+      <c r="O21">
+        <v>0.3</v>
+      </c>
+      <c r="P21">
+        <v>1.92</v>
+      </c>
+      <c r="S21">
+        <v>0.1</v>
+      </c>
+      <c r="T21">
+        <v>0.2</v>
+      </c>
+      <c r="V21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W21">
+        <v>0.3</v>
+      </c>
+      <c r="X21">
+        <v>0.7</v>
+      </c>
+      <c r="AI21">
         <v>5</v>
       </c>
-      <c r="AJ20" t="s">
+      <c r="AK21" t="s">
         <v>1</v>
       </c>
-      <c r="AK20" t="s">
+      <c r="AL21" t="s">
         <v>1</v>
       </c>
-      <c r="AL20">
+      <c r="AM21">
         <v>63</v>
       </c>
-      <c r="AM20">
+      <c r="AN21">
         <v>11</v>
       </c>
-      <c r="AN20">
+      <c r="AO21">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A21">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>42.476743999999897</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>43.21978</v>
       </c>
-      <c r="E21">
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22">
         <v>5.55</v>
       </c>
-      <c r="F21">
+      <c r="G22">
         <v>152.30000000000001</v>
       </c>
-      <c r="G21">
+      <c r="H22">
         <v>0.22</v>
       </c>
-      <c r="H21">
+      <c r="I22">
         <v>0.24</v>
       </c>
-      <c r="J21">
+      <c r="K22">
         <v>2.68</v>
       </c>
-      <c r="K21">
+      <c r="L22">
         <v>0.89</v>
       </c>
-      <c r="L21">
+      <c r="M22">
         <v>1.1299999999999999</v>
       </c>
-      <c r="M21">
+      <c r="N22">
         <v>0.2</v>
       </c>
-      <c r="N21">
+      <c r="O22">
         <v>0.9</v>
       </c>
-      <c r="O21">
+      <c r="P22">
         <v>7.2</v>
       </c>
-      <c r="R21">
+      <c r="S22">
         <v>0.2</v>
       </c>
-      <c r="S21">
+      <c r="T22">
         <v>0.5</v>
       </c>
-      <c r="V21">
+      <c r="W22">
         <v>1.2</v>
       </c>
-      <c r="W21">
+      <c r="X22">
         <v>0.5</v>
       </c>
-      <c r="AH21">
+      <c r="AI22">
         <v>6</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AJ22" t="s">
         <v>0</v>
       </c>
-      <c r="AJ21" t="s">
+      <c r="AK22" t="s">
         <v>0</v>
       </c>
-      <c r="AK21" t="s">
+      <c r="AL22" t="s">
         <v>0</v>
       </c>
-      <c r="AL21">
+      <c r="AM22">
         <v>59</v>
       </c>
-      <c r="AM21">
+      <c r="AN22">
         <v>10</v>
       </c>
-      <c r="AN21">
+      <c r="AO22">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A22">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>42.477587999999898</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>43.216532999999899</v>
       </c>
-      <c r="D22">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23">
         <v>0.5</v>
       </c>
-      <c r="E22">
+      <c r="F23">
         <v>7.86</v>
       </c>
-      <c r="F22">
+      <c r="G23">
         <v>384.6</v>
       </c>
-      <c r="J22">
+      <c r="K23">
         <v>5.0199999999999996</v>
       </c>
-      <c r="K22">
+      <c r="L23">
         <v>0.78</v>
       </c>
-      <c r="L22">
+      <c r="M23">
         <v>0.16</v>
       </c>
-      <c r="N22">
+      <c r="O23">
         <v>3.36</v>
       </c>
-      <c r="O22">
+      <c r="P23">
         <v>2.89</v>
       </c>
-      <c r="Q22">
+      <c r="R23">
         <v>0.6</v>
       </c>
-      <c r="S22">
+      <c r="T23">
         <v>0.8</v>
       </c>
-      <c r="T22">
+      <c r="U23">
         <v>0.2</v>
       </c>
-      <c r="U22">
+      <c r="V23">
         <v>0.9</v>
       </c>
-      <c r="V22">
+      <c r="W23">
         <v>0.3</v>
       </c>
-      <c r="W22">
+      <c r="X23">
         <v>0.8</v>
       </c>
-      <c r="X22">
+      <c r="Y23">
         <v>1.6</v>
       </c>
-      <c r="AH22">
+      <c r="AI23">
         <v>10</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AK23" t="s">
         <v>52</v>
       </c>
-      <c r="AL22">
+      <c r="AM23">
         <v>56</v>
       </c>
-      <c r="AM22">
+      <c r="AN23">
         <v>13</v>
       </c>
-      <c r="AN22">
+      <c r="AO23">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>42.478431</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>43.215865000000001</v>
       </c>
-      <c r="D23">
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24">
         <v>0.35</v>
       </c>
-      <c r="E23">
+      <c r="F24">
         <v>5.07</v>
       </c>
-      <c r="F23">
+      <c r="G24">
         <v>234.3</v>
       </c>
-      <c r="J23">
+      <c r="K24">
         <v>4.95</v>
       </c>
-      <c r="K23">
+      <c r="L24">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L23">
+      <c r="M24">
         <v>0.11</v>
       </c>
-      <c r="N23">
+      <c r="O24">
         <v>0.4</v>
       </c>
-      <c r="O23">
+      <c r="P24">
         <v>1.36</v>
       </c>
-      <c r="Q23">
+      <c r="R24">
         <v>0.1</v>
       </c>
-      <c r="R23">
+      <c r="S24">
         <v>0.2</v>
       </c>
-      <c r="S23">
+      <c r="T24">
         <v>0.15</v>
       </c>
-      <c r="U23">
+      <c r="V24">
         <v>0.6</v>
       </c>
-      <c r="V23">
+      <c r="W24">
         <v>0.4</v>
       </c>
-      <c r="W23">
+      <c r="X24">
         <v>0.9</v>
       </c>
-      <c r="AB23">
+      <c r="AC24">
         <v>0.4</v>
       </c>
-      <c r="AH23">
+      <c r="AI24">
         <v>9</v>
       </c>
-      <c r="AJ23" t="s">
+      <c r="AK24" t="s">
         <v>51</v>
       </c>
-      <c r="AL23">
+      <c r="AM24">
         <v>46</v>
       </c>
-      <c r="AM23">
+      <c r="AN24">
         <v>15</v>
       </c>
-      <c r="AN23">
+      <c r="AO24">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>42.480438999999897</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>43.218026000000002</v>
       </c>
-      <c r="D24">
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25">
         <v>0.38</v>
       </c>
-      <c r="E24">
+      <c r="F25">
         <v>4.55</v>
       </c>
-      <c r="F24">
+      <c r="G25">
         <v>203.1</v>
       </c>
-      <c r="J24">
+      <c r="K25">
         <v>6.91</v>
       </c>
-      <c r="K24">
+      <c r="L25">
         <v>0.71</v>
       </c>
-      <c r="L24">
+      <c r="M25">
         <v>1.01</v>
       </c>
-      <c r="M24">
+      <c r="N25">
         <v>0.1</v>
       </c>
-      <c r="N24">
+      <c r="O25">
         <v>0.1</v>
       </c>
-      <c r="O24">
+      <c r="P25">
         <v>1.82</v>
       </c>
-      <c r="Q24">
+      <c r="R25">
         <v>0.3</v>
       </c>
-      <c r="S24">
+      <c r="T25">
         <v>0.3</v>
       </c>
-      <c r="U24">
+      <c r="V25">
         <v>1.2</v>
       </c>
-      <c r="V24">
+      <c r="W25">
         <v>0.7</v>
       </c>
-      <c r="W24">
+      <c r="X25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Z24">
+      <c r="AA25">
         <v>0.15</v>
       </c>
-      <c r="AH24">
+      <c r="AI25">
         <v>3</v>
       </c>
-      <c r="AJ24" t="s">
+      <c r="AK25" t="s">
         <v>0</v>
       </c>
-      <c r="AL24">
+      <c r="AM25">
         <v>69</v>
       </c>
-      <c r="AM24">
+      <c r="AN25">
         <v>8</v>
       </c>
-      <c r="AN24">
+      <c r="AO25">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>42.484884999999899</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>43.217697000000001</v>
       </c>
-      <c r="D25">
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26">
         <v>0.69</v>
       </c>
-      <c r="E25">
+      <c r="F26">
         <v>8.67</v>
       </c>
-      <c r="F25">
+      <c r="G26">
         <v>238.5</v>
       </c>
-      <c r="J25">
+      <c r="K26">
         <v>5.91</v>
       </c>
-      <c r="K25">
+      <c r="L26">
         <v>0.24</v>
       </c>
-      <c r="L25">
+      <c r="M26">
         <v>0.26</v>
       </c>
-      <c r="M25">
+      <c r="N26">
         <v>0.1</v>
       </c>
-      <c r="N25">
+      <c r="O26">
         <v>0.2</v>
       </c>
-      <c r="O25">
+      <c r="P26">
         <v>2.04</v>
       </c>
-      <c r="S25">
+      <c r="T26">
         <v>0.3</v>
-      </c>
-      <c r="V25">
-        <v>0.7</v>
-      </c>
-      <c r="W25">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AB25">
-        <v>0.5</v>
-      </c>
-      <c r="AH25">
-        <v>23</v>
-      </c>
-      <c r="AJ25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL25">
-        <v>51</v>
-      </c>
-      <c r="AM25">
-        <v>4</v>
-      </c>
-      <c r="AN25">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>42.486913999999899</v>
-      </c>
-      <c r="C26">
-        <v>43.2182859999999</v>
-      </c>
-      <c r="D26">
-        <v>0.52</v>
-      </c>
-      <c r="E26">
-        <v>4.76</v>
-      </c>
-      <c r="F26">
-        <v>209.3</v>
-      </c>
-      <c r="J26">
-        <v>5.2</v>
-      </c>
-      <c r="K26">
-        <v>0.87</v>
-      </c>
-      <c r="L26">
-        <v>0.32</v>
-      </c>
-      <c r="N26">
-        <v>0.6</v>
-      </c>
-      <c r="O26">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="P26">
-        <v>0.5</v>
-      </c>
-      <c r="S26">
-        <v>0.4</v>
-      </c>
-      <c r="V26">
-        <v>0.6</v>
       </c>
       <c r="W26">
         <v>0.7</v>
       </c>
-      <c r="Z26">
+      <c r="X26">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AC26">
+        <v>0.5</v>
+      </c>
+      <c r="AI26">
+        <v>23</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM26">
+        <v>51</v>
+      </c>
+      <c r="AN26">
+        <v>4</v>
+      </c>
+      <c r="AO26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>42.486913999999899</v>
+      </c>
+      <c r="C27">
+        <v>43.2182859999999</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27">
+        <v>0.52</v>
+      </c>
+      <c r="F27">
+        <v>4.76</v>
+      </c>
+      <c r="G27">
+        <v>209.3</v>
+      </c>
+      <c r="K27">
+        <v>5.2</v>
+      </c>
+      <c r="L27">
+        <v>0.87</v>
+      </c>
+      <c r="M27">
+        <v>0.32</v>
+      </c>
+      <c r="O27">
+        <v>0.6</v>
+      </c>
+      <c r="P27">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Q27">
+        <v>0.5</v>
+      </c>
+      <c r="T27">
+        <v>0.4</v>
+      </c>
+      <c r="W27">
+        <v>0.6</v>
+      </c>
+      <c r="X27">
+        <v>0.7</v>
+      </c>
+      <c r="AA27">
         <v>0.9</v>
       </c>
-      <c r="AH26">
+      <c r="AI27">
         <v>20</v>
       </c>
-      <c r="AJ26" t="s">
+      <c r="AK27" t="s">
         <v>52</v>
       </c>
-      <c r="AL26">
+      <c r="AM27">
         <v>43</v>
       </c>
-      <c r="AM26">
+      <c r="AN27">
         <v>8</v>
       </c>
-      <c r="AN26">
+      <c r="AO27">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>42.487506000000003</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>43.218822000000003</v>
       </c>
-      <c r="D27">
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28">
         <v>0.46</v>
       </c>
-      <c r="E27">
+      <c r="F28">
         <v>8.8800000000000008</v>
       </c>
-      <c r="F27">
+      <c r="G28">
         <v>166</v>
       </c>
-      <c r="J27">
+      <c r="K28">
         <v>10.029999999999999</v>
       </c>
-      <c r="K27">
+      <c r="L28">
         <v>0.21</v>
       </c>
-      <c r="L27">
+      <c r="M28">
         <v>0.69</v>
       </c>
-      <c r="N27">
+      <c r="O28">
         <v>0.3</v>
       </c>
-      <c r="O27">
+      <c r="P28">
         <v>2.11</v>
-      </c>
-      <c r="R27">
-        <v>0.4</v>
-      </c>
-      <c r="S27">
-        <v>0.2</v>
-      </c>
-      <c r="V27">
-        <v>0.8</v>
-      </c>
-      <c r="W27">
-        <v>1.7</v>
-      </c>
-      <c r="X27">
-        <v>0.15</v>
-      </c>
-      <c r="Y27">
-        <v>0.5</v>
-      </c>
-      <c r="AB27">
-        <v>0.8</v>
-      </c>
-      <c r="AH27">
-        <v>6</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL27">
-        <v>59</v>
-      </c>
-      <c r="AM27">
-        <v>10</v>
-      </c>
-      <c r="AN27">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>42.478547880400001</v>
-      </c>
-      <c r="C28">
-        <v>43.217169552100003</v>
-      </c>
-      <c r="E28">
-        <v>8.48</v>
-      </c>
-      <c r="F28">
-        <v>224.9</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>6.51</v>
-      </c>
-      <c r="K28">
-        <v>0.38</v>
-      </c>
-      <c r="L28">
-        <v>0.19</v>
-      </c>
-      <c r="M28">
-        <v>0.1</v>
-      </c>
-      <c r="N28">
-        <v>0.4</v>
-      </c>
-      <c r="O28">
-        <v>2.38</v>
-      </c>
-      <c r="P28">
-        <v>0.3</v>
-      </c>
-      <c r="Q28">
-        <v>0.1</v>
-      </c>
-      <c r="R28">
-        <v>0.4</v>
       </c>
       <c r="S28">
         <v>0.4</v>
       </c>
-      <c r="V28">
+      <c r="T28">
+        <v>0.2</v>
+      </c>
+      <c r="W28">
+        <v>0.8</v>
+      </c>
+      <c r="X28">
+        <v>1.7</v>
+      </c>
+      <c r="Y28">
+        <v>0.15</v>
+      </c>
+      <c r="Z28">
         <v>0.5</v>
       </c>
-      <c r="W28">
+      <c r="AC28">
+        <v>0.8</v>
+      </c>
+      <c r="AI28">
+        <v>6</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM28">
+        <v>59</v>
+      </c>
+      <c r="AN28">
+        <v>10</v>
+      </c>
+      <c r="AO28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>42.478547880400001</v>
+      </c>
+      <c r="C29">
+        <v>43.217169552100003</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29">
+        <v>8.48</v>
+      </c>
+      <c r="G29">
+        <v>224.9</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>6.51</v>
+      </c>
+      <c r="L29">
+        <v>0.38</v>
+      </c>
+      <c r="M29">
+        <v>0.19</v>
+      </c>
+      <c r="N29">
+        <v>0.1</v>
+      </c>
+      <c r="O29">
+        <v>0.4</v>
+      </c>
+      <c r="P29">
+        <v>2.38</v>
+      </c>
+      <c r="Q29">
+        <v>0.3</v>
+      </c>
+      <c r="R29">
+        <v>0.1</v>
+      </c>
+      <c r="S29">
+        <v>0.4</v>
+      </c>
+      <c r="T29">
+        <v>0.4</v>
+      </c>
+      <c r="W29">
+        <v>0.5</v>
+      </c>
+      <c r="X29">
         <v>0.7</v>
       </c>
-      <c r="AH28">
+      <c r="AI29">
         <v>6</v>
       </c>
-      <c r="AJ28" t="s">
+      <c r="AK29" t="s">
         <v>51</v>
       </c>
-      <c r="AK28" t="s">
+      <c r="AL29" t="s">
         <v>52</v>
       </c>
-      <c r="AL28">
+      <c r="AM29">
         <v>63</v>
       </c>
-      <c r="AM28">
+      <c r="AN29">
         <v>6</v>
       </c>
-      <c r="AN28">
+      <c r="AO29">
         <v>19</v>
       </c>
-      <c r="AO28">
+      <c r="AP29">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>42.481013966600003</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>43.219298332500003</v>
       </c>
-      <c r="D29">
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30">
         <v>1.02</v>
       </c>
-      <c r="E29">
+      <c r="F30">
         <v>2.8</v>
       </c>
-      <c r="F29">
+      <c r="G30">
         <v>128.9</v>
       </c>
-      <c r="J29">
+      <c r="K30">
         <v>2.31</v>
       </c>
-      <c r="K29">
+      <c r="L30">
         <v>1.89</v>
       </c>
-      <c r="L29">
+      <c r="M30">
         <v>0.52</v>
       </c>
-      <c r="M29">
+      <c r="N30">
         <v>0.4</v>
       </c>
-      <c r="N29">
+      <c r="O30">
         <v>0.5</v>
       </c>
-      <c r="O29">
+      <c r="P30">
         <v>3.84</v>
       </c>
-      <c r="S29">
+      <c r="T30">
         <v>1.4</v>
       </c>
-      <c r="U29">
+      <c r="V30">
         <v>0.26</v>
       </c>
-      <c r="V29">
+      <c r="W30">
         <v>0.7</v>
       </c>
-      <c r="W29">
+      <c r="X30">
         <v>1.2</v>
       </c>
-      <c r="AH29">
+      <c r="AI30">
         <v>5</v>
       </c>
-      <c r="AJ29" t="s">
+      <c r="AK30" t="s">
         <v>54</v>
       </c>
-      <c r="AK29" t="s">
+      <c r="AL30" t="s">
         <v>0</v>
       </c>
-      <c r="AL29">
+      <c r="AM30">
         <v>48</v>
       </c>
-      <c r="AM29">
+      <c r="AN30">
         <v>8</v>
       </c>
-      <c r="AN29">
+      <c r="AO30">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>2019</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B31" s="3">
         <v>42.487691000439384</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C31" s="3">
         <v>43.218566000120859</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="3">
         <v>0.87</v>
       </c>
-      <c r="E30" s="3">
+      <c r="F31" s="3">
         <v>43.4</v>
       </c>
-      <c r="F30" s="3">
+      <c r="G31" s="3">
         <v>259</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="J30" s="3">
-        <v>47.34</v>
-      </c>
-      <c r="K30" s="3">
-        <v>3.45</v>
-      </c>
-      <c r="L30" s="3">
-        <v>0.94</v>
-      </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3">
-        <v>0.85</v>
-      </c>
-      <c r="O30" s="3">
-        <v>21.2</v>
-      </c>
-      <c r="P30" s="3">
-        <v>0.53300000000000003</v>
-      </c>
-      <c r="Q30" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3">
-        <v>0.74</v>
-      </c>
-      <c r="W30" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
-      <c r="AE30" s="3"/>
-      <c r="AF30" s="3"/>
-      <c r="AG30" s="3"/>
-      <c r="AH30" s="3">
-        <v>10</v>
-      </c>
-      <c r="AI30" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="3">
-        <v>2</v>
-      </c>
-      <c r="AK30" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="3">
-        <v>53</v>
-      </c>
-      <c r="AM30" s="3">
-        <v>11</v>
-      </c>
-      <c r="AN30" s="3">
-        <v>24</v>
-      </c>
-      <c r="AO30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
-        <v>2020</v>
-      </c>
-      <c r="B31" s="3">
-        <v>42.487632000416511</v>
-      </c>
-      <c r="C31" s="3">
-        <v>43.21873199968212</v>
-      </c>
-      <c r="D31" s="3">
-        <v>10.69</v>
-      </c>
-      <c r="E31" s="3">
-        <v>109.44</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1.05</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3">
-        <v>107.2</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="K31" s="3">
-        <v>3.78</v>
+        <v>47.34</v>
       </c>
       <c r="L31" s="3">
-        <v>4.7699999999999996</v>
+        <v>3.45</v>
       </c>
       <c r="M31" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="N31" s="3">
-        <v>5.19</v>
-      </c>
+        <v>0.94</v>
+      </c>
+      <c r="N31" s="3"/>
       <c r="O31" s="3">
-        <v>36.75</v>
-      </c>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
+        <v>0.85</v>
+      </c>
+      <c r="P31" s="3">
+        <v>21.2</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.53300000000000003</v>
+      </c>
       <c r="R31" s="3">
         <v>0.32</v>
       </c>
-      <c r="S31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="T31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="U31" s="3"/>
-      <c r="V31" s="3">
-        <v>0.55000000000000004</v>
-      </c>
+      <c r="V31" s="3"/>
       <c r="W31" s="3">
-        <v>2.7850000000000001</v>
-      </c>
-      <c r="X31" s="3"/>
+        <v>0.74</v>
+      </c>
+      <c r="X31" s="3">
+        <v>1.99</v>
+      </c>
       <c r="Y31" s="3"/>
-      <c r="Z31" s="3">
-        <v>1.1499999999999999</v>
-      </c>
+      <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
@@ -2869,211 +2952,316 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
-      <c r="AH31" s="3">
-        <v>16</v>
-      </c>
+      <c r="AH31" s="3"/>
       <c r="AI31" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="3">
         <v>2</v>
       </c>
-      <c r="AJ31" s="3">
-        <v>4</v>
-      </c>
-      <c r="AK31" s="3">
+      <c r="AL31" s="3">
         <v>0</v>
       </c>
-      <c r="AL31" s="3">
-        <v>45</v>
-      </c>
       <c r="AM31" s="3">
+        <v>53</v>
+      </c>
+      <c r="AN31" s="3">
         <v>11</v>
       </c>
-      <c r="AN31" s="3">
-        <v>22</v>
-      </c>
       <c r="AO31" s="3">
+        <v>24</v>
+      </c>
+      <c r="AP31" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B32" s="3">
-        <v>42.489012000203672</v>
+        <v>42.487632000416511</v>
       </c>
       <c r="C32" s="3">
-        <v>43.219430000394247</v>
-      </c>
-      <c r="D32" s="3">
-        <v>6.5</v>
+        <v>43.21873199968212</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
       </c>
       <c r="E32" s="3">
-        <v>74.56</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+        <v>10.69</v>
+      </c>
+      <c r="F32" s="3">
+        <v>109.44</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1.05</v>
+      </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="3">
-        <v>81.739999999999995</v>
-      </c>
+      <c r="J32" s="3"/>
       <c r="K32" s="3">
-        <v>12.05</v>
+        <v>107.2</v>
       </c>
       <c r="L32" s="3">
-        <v>1.96</v>
+        <v>3.78</v>
       </c>
       <c r="M32" s="3">
-        <v>0.16500000000000001</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="N32" s="3">
-        <v>0.43</v>
+        <v>0.22</v>
       </c>
       <c r="O32" s="3">
-        <v>19.47</v>
-      </c>
-      <c r="P32" s="3"/>
+        <v>5.19</v>
+      </c>
+      <c r="P32" s="3">
+        <v>36.75</v>
+      </c>
       <c r="Q32" s="3"/>
-      <c r="R32" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="S32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T32" s="3">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="U32" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="V32" s="3">
-        <v>0.61</v>
-      </c>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="T32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
       <c r="W32" s="3">
-        <v>3.23</v>
-      </c>
-      <c r="X32" s="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="X32" s="3">
+        <v>2.7850000000000001</v>
+      </c>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
-      <c r="AA32" s="3"/>
+      <c r="AA32" s="3">
+        <v>1.1499999999999999</v>
+      </c>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
-      <c r="AH32" s="3">
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3">
+        <v>16</v>
+      </c>
+      <c r="AJ32" s="3">
+        <v>2</v>
+      </c>
+      <c r="AK32" s="3">
+        <v>4</v>
+      </c>
+      <c r="AL32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="3">
+        <v>45</v>
+      </c>
+      <c r="AN32" s="3">
+        <v>11</v>
+      </c>
+      <c r="AO32" s="3">
+        <v>22</v>
+      </c>
+      <c r="AP32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B33" s="3">
+        <v>42.489012000203672</v>
+      </c>
+      <c r="C33" s="3">
+        <v>43.219430000394247</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="F33" s="3">
+        <v>74.56</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3">
+        <v>81.739999999999995</v>
+      </c>
+      <c r="L33" s="3">
+        <v>12.05</v>
+      </c>
+      <c r="M33" s="3">
+        <v>1.96</v>
+      </c>
+      <c r="N33" s="3">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="P33" s="3">
+        <v>19.47</v>
+      </c>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U33" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="V33" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="W33" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="X33" s="3">
+        <v>3.23</v>
+      </c>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3">
         <v>17</v>
       </c>
-      <c r="AI32" s="3">
+      <c r="AJ33" s="3">
         <v>0</v>
       </c>
-      <c r="AJ32" s="3">
+      <c r="AK33" s="3">
         <v>1</v>
       </c>
-      <c r="AK32" s="3">
+      <c r="AL33" s="3">
         <v>0</v>
       </c>
-      <c r="AL32" s="3">
+      <c r="AM33" s="3">
         <v>58</v>
       </c>
-      <c r="AM32" s="3">
+      <c r="AN33" s="3">
         <v>9</v>
       </c>
-      <c r="AN32" s="3">
+      <c r="AO33" s="3">
         <v>15</v>
       </c>
-      <c r="AO32" s="3">
+      <c r="AP33" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>3000</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="2">
         <v>42.489991000000003</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>43.22139</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2">
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2">
         <v>5.09</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G34" s="2">
         <v>424.8</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2">
         <v>7.45</v>
       </c>
-      <c r="K33" s="2">
+      <c r="L34" s="2">
         <v>2.57</v>
       </c>
-      <c r="L33" s="2">
+      <c r="M34" s="2">
         <v>0.72</v>
       </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2">
+      <c r="N34" s="2"/>
+      <c r="O34" s="2">
         <v>0.8</v>
       </c>
-      <c r="O33" s="2">
+      <c r="P34" s="2">
         <v>3.19</v>
       </c>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2">
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2">
         <v>0.4</v>
       </c>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2">
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2">
         <v>0.4</v>
       </c>
-      <c r="W33" s="2">
+      <c r="X34" s="2">
         <v>1.7</v>
       </c>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-      <c r="AA33" s="2">
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2">
         <v>0.11</v>
       </c>
-      <c r="AB33" s="2"/>
-      <c r="AC33" s="2"/>
-      <c r="AD33" s="2"/>
-      <c r="AE33" s="2"/>
-      <c r="AF33" s="2"/>
-      <c r="AG33" s="2"/>
-      <c r="AH33" s="2">
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2">
         <v>15</v>
       </c>
-      <c r="AI33" s="2" t="s">
+      <c r="AJ34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AJ33" s="2" t="s">
+      <c r="AK34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AK33" s="2"/>
-      <c r="AL33" s="2">
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2">
         <v>50</v>
       </c>
-      <c r="AM33" s="2">
+      <c r="AN34" s="2">
         <v>13</v>
       </c>
-      <c r="AN33" s="2">
+      <c r="AO34" s="2">
         <v>19</v>
       </c>
-      <c r="AO33" s="2"/>
-      <c r="AP33" s="2"/>
-      <c r="AQ33" s="2"/>
-      <c r="AR33" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>